<commit_message>
ann - var_mc sens var formula bugfix
</commit_message>
<xml_diff>
--- a/qf609-risk-analysis/data/SwapPricingExample.xlsx
+++ b/qf609-risk-analysis/data/SwapPricingExample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Desktop/qf609/project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Desktop/qf609/project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9088CB99-CCD4-A343-B7B0-C450ED37446F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5FA684-BC7B-8E49-AF54-D3A35B7B0226}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1780" yWindow="500" windowWidth="24700" windowHeight="16780" activeTab="1" xr2:uid="{1A4CF143-4BD9-4BB1-B9E1-9D07161B787B}"/>
   </bookViews>
@@ -251,15 +251,23 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="dd/mmm/yyyy"/>
     <numFmt numFmtId="166" formatCode="#,##0_ ;\-#,##0\ "/>
     <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="172" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -468,10 +476,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -512,7 +520,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -540,8 +548,8 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -550,50 +558,53 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1194,7 +1205,7 @@
         <v>1</v>
       </c>
       <c r="O9" s="22">
-        <f t="shared" ref="O8:O17" si="0">$J$6*$J$8*0.5</f>
+        <f t="shared" ref="O9:O17" si="0">$J$6*$J$8*0.5</f>
         <v>19000</v>
       </c>
       <c r="P9" s="20">
@@ -1202,11 +1213,11 @@
         <v>0.04</v>
       </c>
       <c r="Q9" s="20">
-        <f t="shared" ref="Q8:Q17" si="1">EXP(-P9*N9)</f>
+        <f t="shared" ref="Q9:Q17" si="1">EXP(-P9*N9)</f>
         <v>0.96078943915232318</v>
       </c>
       <c r="R9" s="16">
-        <f t="shared" ref="R8:R17" si="2">Q9*O9</f>
+        <f t="shared" ref="R9:R17" si="2">Q9*O9</f>
         <v>18254.999343894142</v>
       </c>
       <c r="S9" s="1"/>
@@ -1230,19 +1241,19 @@
         <v>0.98019867330675525</v>
       </c>
       <c r="Z9" s="20">
-        <f t="shared" ref="Z8:Z17" si="5">EXP(-X9*V9)</f>
+        <f t="shared" ref="Z9:Z17" si="5">EXP(-X9*V9)</f>
         <v>0.96078943915232318</v>
       </c>
       <c r="AA9" s="26">
-        <f t="shared" ref="AA8:AA17" si="6">1/0.5*(Y9/Z9-1)</f>
+        <f t="shared" ref="AA9:AA17" si="6">1/0.5*(Y9/Z9-1)</f>
         <v>4.0402680053511553E-2</v>
       </c>
       <c r="AB9" s="22">
-        <f t="shared" ref="AB8:AB17" si="7">$J$6*AA9*0.5</f>
+        <f t="shared" ref="AB9:AB17" si="7">$J$6*AA9*0.5</f>
         <v>20201.340026755777</v>
       </c>
       <c r="AC9" s="16">
-        <f t="shared" ref="AC8:AC17" si="8">AB9*Z9</f>
+        <f t="shared" ref="AC9:AC17" si="8">AB9*Z9</f>
         <v>19409.234154432059</v>
       </c>
     </row>
@@ -1293,7 +1304,7 @@
         <v>1.5</v>
       </c>
       <c r="W10" s="20">
-        <f t="shared" ref="W9:W17" si="9">X9</f>
+        <f t="shared" ref="W10:W17" si="9">X9</f>
         <v>0.04</v>
       </c>
       <c r="X10" s="20">
@@ -2059,10 +2070,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EDFB715-35B2-6541-B5AA-91BEBA61F75D}">
-  <dimension ref="A1:Q36"/>
+  <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2077,10 +2088,14 @@
     <col min="14" max="14" width="10.83203125" style="30"/>
     <col min="15" max="15" width="21.5" style="30" customWidth="1"/>
     <col min="16" max="16" width="14" style="30" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="30"/>
+    <col min="17" max="19" width="10.83203125" style="30"/>
+    <col min="20" max="20" width="13" style="30" customWidth="1"/>
+    <col min="21" max="21" width="10.83203125" style="30"/>
+    <col min="22" max="22" width="12.83203125" style="30" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="10.83203125" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:22">
       <c r="A1" s="36" t="s">
         <v>1</v>
       </c>
@@ -2121,7 +2136,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:22">
       <c r="A2" s="33">
         <v>1</v>
       </c>
@@ -2129,25 +2144,25 @@
         <v>5.22446062245015E-2</v>
       </c>
       <c r="C2" s="33">
-        <f>EXP(-B2*A2)</f>
+        <f t="shared" ref="C2:C11" si="0">EXP(-B2*A2)</f>
         <v>0.94909668349086507</v>
       </c>
       <c r="D2" s="39">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E2" s="40">
-        <f>100*1000000*D2</f>
+        <f t="shared" ref="E2:E11" si="1">100*1000000*D2</f>
         <v>4200000</v>
       </c>
       <c r="F2" s="41">
-        <f>C2*E2</f>
+        <f t="shared" ref="F2:F11" si="2">C2*E2</f>
         <v>3986206.0706616333</v>
       </c>
       <c r="G2" s="30">
         <v>0.04</v>
       </c>
       <c r="H2" s="30">
-        <f>B2</f>
+        <f t="shared" ref="H2:H11" si="3">B2</f>
         <v>5.22446062245015E-2</v>
       </c>
       <c r="I2" s="33">
@@ -2155,23 +2170,23 @@
         <v>1</v>
       </c>
       <c r="J2" s="33">
-        <f>EXP(-A2*H2)</f>
+        <f t="shared" ref="J2:J11" si="4">EXP(-A2*H2)</f>
         <v>0.94909668349086507</v>
       </c>
       <c r="K2" s="43">
-        <f>(I2-J2)/J2</f>
+        <f t="shared" ref="K2:K11" si="5">(I2-J2)/J2</f>
         <v>5.3633436292188738E-2</v>
       </c>
       <c r="L2" s="40">
-        <f>100*1000000*K2</f>
+        <f t="shared" ref="L2:L11" si="6">100*1000000*K2</f>
         <v>5363343.6292188736</v>
       </c>
       <c r="M2" s="41">
-        <f>L2*J2</f>
+        <f t="shared" ref="M2:M11" si="7">L2*J2</f>
         <v>5090331.6509134928</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:22">
       <c r="A3" s="33">
         <v>2</v>
       </c>
@@ -2179,50 +2194,50 @@
         <v>4.7904200566131802E-2</v>
       </c>
       <c r="C3" s="33">
-        <f>EXP(-B3*A3)</f>
+        <f t="shared" si="0"/>
         <v>0.90863809342154345</v>
       </c>
       <c r="D3" s="39">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E3" s="40">
-        <f>100*1000000*D3</f>
+        <f t="shared" si="1"/>
         <v>4200000</v>
       </c>
       <c r="F3" s="41">
-        <f>C3*E3</f>
+        <f t="shared" si="2"/>
         <v>3816279.9923704825</v>
       </c>
       <c r="G3" s="30">
-        <f>B2</f>
+        <f t="shared" ref="G3:G11" si="8">B2</f>
         <v>5.22446062245015E-2</v>
       </c>
       <c r="H3" s="30">
-        <f>B3</f>
+        <f t="shared" si="3"/>
         <v>4.7904200566131802E-2</v>
       </c>
       <c r="I3" s="33">
-        <f>J2</f>
+        <f t="shared" ref="I3:I11" si="9">J2</f>
         <v>0.94909668349086507</v>
       </c>
       <c r="J3" s="33">
-        <f>EXP(-A3*H3)</f>
+        <f t="shared" si="4"/>
         <v>0.90863809342154345</v>
       </c>
       <c r="K3" s="43">
-        <f>(I3-J3)/J3</f>
+        <f t="shared" si="5"/>
         <v>4.4526627666436294E-2</v>
       </c>
       <c r="L3" s="40">
-        <f>100*1000000*K3</f>
+        <f t="shared" si="6"/>
         <v>4452662.7666436294</v>
       </c>
       <c r="M3" s="41">
-        <f>L3*J3</f>
+        <f t="shared" si="7"/>
         <v>4045859.0069321622</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:22">
       <c r="A4" s="33">
         <v>3</v>
       </c>
@@ -2230,50 +2245,50 @@
         <v>4.5429337602591303E-2</v>
       </c>
       <c r="C4" s="33">
-        <f>EXP(-B4*A4)</f>
+        <f t="shared" si="0"/>
         <v>0.87259127882966547</v>
       </c>
       <c r="D4" s="39">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E4" s="40">
-        <f>100*1000000*D4</f>
+        <f t="shared" si="1"/>
         <v>4200000</v>
       </c>
       <c r="F4" s="41">
-        <f>C4*E4</f>
+        <f t="shared" si="2"/>
         <v>3664883.3710845951</v>
       </c>
       <c r="G4" s="30">
-        <f>B3</f>
+        <f t="shared" si="8"/>
         <v>4.7904200566131802E-2</v>
       </c>
       <c r="H4" s="30">
-        <f>B4</f>
+        <f t="shared" si="3"/>
         <v>4.5429337602591303E-2</v>
       </c>
       <c r="I4" s="33">
-        <f>J3</f>
+        <f t="shared" si="9"/>
         <v>0.90863809342154345</v>
       </c>
       <c r="J4" s="33">
-        <f>EXP(-A4*H4)</f>
+        <f t="shared" si="4"/>
         <v>0.87259127882966547</v>
       </c>
       <c r="K4" s="43">
-        <f>(I4-J4)/J4</f>
+        <f t="shared" si="5"/>
         <v>4.131007891830478E-2</v>
       </c>
       <c r="L4" s="40">
-        <f>100*1000000*K4</f>
+        <f t="shared" si="6"/>
         <v>4131007.8918304779</v>
       </c>
       <c r="M4" s="41">
-        <f>L4*J4</f>
+        <f t="shared" si="7"/>
         <v>3604681.4591877973</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:22">
       <c r="A5" s="33">
         <v>4</v>
       </c>
@@ -2281,50 +2296,50 @@
         <v>4.4344750256342602E-2</v>
       </c>
       <c r="C5" s="33">
-        <f>EXP(-B5*A5)</f>
+        <f t="shared" si="0"/>
         <v>0.83746232528811282</v>
       </c>
       <c r="D5" s="39">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E5" s="40">
-        <f>100*1000000*D5</f>
+        <f t="shared" si="1"/>
         <v>4200000</v>
       </c>
       <c r="F5" s="41">
-        <f>C5*E5</f>
+        <f t="shared" si="2"/>
         <v>3517341.7662100741</v>
       </c>
       <c r="G5" s="30">
-        <f>B4</f>
+        <f t="shared" si="8"/>
         <v>4.5429337602591303E-2</v>
       </c>
       <c r="H5" s="30">
-        <f>B5</f>
+        <f t="shared" si="3"/>
         <v>4.4344750256342602E-2</v>
       </c>
       <c r="I5" s="33">
-        <f>J4</f>
+        <f t="shared" si="9"/>
         <v>0.87259127882966547</v>
       </c>
       <c r="J5" s="33">
-        <f>EXP(-A5*H5)</f>
+        <f t="shared" si="4"/>
         <v>0.83746232528811282</v>
       </c>
       <c r="K5" s="43">
-        <f>(I5-J5)/J5</f>
+        <f t="shared" si="5"/>
         <v>4.1946906124364712E-2</v>
       </c>
       <c r="L5" s="40">
-        <f>100*1000000*K5</f>
+        <f t="shared" si="6"/>
         <v>4194690.6124364715</v>
       </c>
       <c r="M5" s="41">
-        <f>L5*J5</f>
+        <f t="shared" si="7"/>
         <v>3512895.3541552653</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:22">
       <c r="A6" s="34">
         <v>5</v>
       </c>
@@ -2332,50 +2347,50 @@
         <v>4.3927974682530103E-2</v>
       </c>
       <c r="C6" s="34">
-        <f>EXP(-B6*A6)</f>
+        <f t="shared" si="0"/>
         <v>0.80280785836451651</v>
       </c>
       <c r="D6" s="39">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E6" s="40">
-        <f>100*1000000*D6</f>
+        <f t="shared" si="1"/>
         <v>4200000</v>
       </c>
       <c r="F6" s="42">
-        <f>C6*E6</f>
+        <f t="shared" si="2"/>
         <v>3371793.0051309695</v>
       </c>
       <c r="G6" s="30">
-        <f>B5</f>
+        <f t="shared" si="8"/>
         <v>4.4344750256342602E-2</v>
       </c>
       <c r="H6" s="30">
-        <f>B6</f>
+        <f t="shared" si="3"/>
         <v>4.3927974682530103E-2</v>
       </c>
       <c r="I6" s="33">
-        <f>J5</f>
+        <f t="shared" si="9"/>
         <v>0.83746232528811282</v>
       </c>
       <c r="J6" s="33">
-        <f>EXP(-A6*H6)</f>
+        <f t="shared" si="4"/>
         <v>0.80280785836451651</v>
       </c>
       <c r="K6" s="43">
-        <f>(I6-J6)/J6</f>
+        <f t="shared" si="5"/>
         <v>4.3166576612982496E-2</v>
       </c>
       <c r="L6" s="40">
-        <f>100*1000000*K6</f>
+        <f t="shared" si="6"/>
         <v>4316657.6612982498</v>
       </c>
       <c r="M6" s="41">
-        <f>L6*J6</f>
+        <f t="shared" si="7"/>
         <v>3465446.6923596305</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:22">
       <c r="A7" s="34">
         <v>6</v>
       </c>
@@ -2383,50 +2398,50 @@
         <v>4.3794001970382003E-2</v>
       </c>
       <c r="C7" s="34">
-        <f>EXP(-B7*A7)</f>
+        <f t="shared" si="0"/>
         <v>0.76892333271809798</v>
       </c>
       <c r="D7" s="39">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E7" s="40">
-        <f>100*1000000*D7</f>
+        <f t="shared" si="1"/>
         <v>4200000</v>
       </c>
       <c r="F7" s="42">
-        <f>C7*E7</f>
+        <f t="shared" si="2"/>
         <v>3229477.9974160115</v>
       </c>
       <c r="G7" s="30">
-        <f>B6</f>
+        <f t="shared" si="8"/>
         <v>4.3927974682530103E-2</v>
       </c>
       <c r="H7" s="30">
-        <f>B7</f>
+        <f t="shared" si="3"/>
         <v>4.3794001970382003E-2</v>
       </c>
       <c r="I7" s="33">
-        <f>J6</f>
+        <f t="shared" si="9"/>
         <v>0.80280785836451651</v>
       </c>
       <c r="J7" s="33">
-        <f>EXP(-A7*H7)</f>
+        <f t="shared" si="4"/>
         <v>0.76892333271809798</v>
       </c>
       <c r="K7" s="43">
-        <f>(I7-J7)/J7</f>
+        <f t="shared" si="5"/>
         <v>4.4067495684698185E-2</v>
       </c>
       <c r="L7" s="40">
-        <f>100*1000000*K7</f>
+        <f t="shared" si="6"/>
         <v>4406749.5684698187</v>
       </c>
       <c r="M7" s="41">
-        <f>L7*J7</f>
+        <f t="shared" si="7"/>
         <v>3388452.5646418533</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:22">
       <c r="A8" s="34">
         <v>7</v>
       </c>
@@ -2434,50 +2449,50 @@
         <v>4.3779352153421297E-2</v>
       </c>
       <c r="C8" s="34">
-        <f>EXP(-B8*A8)</f>
+        <f t="shared" si="0"/>
         <v>0.73605129743954478</v>
       </c>
       <c r="D8" s="39">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E8" s="40">
-        <f>100*1000000*D8</f>
+        <f t="shared" si="1"/>
         <v>4200000</v>
       </c>
       <c r="F8" s="42">
-        <f>C8*E8</f>
+        <f t="shared" si="2"/>
         <v>3091415.449246088</v>
       </c>
       <c r="G8" s="30">
-        <f>B7</f>
+        <f t="shared" si="8"/>
         <v>4.3794001970382003E-2</v>
       </c>
       <c r="H8" s="30">
-        <f>B8</f>
+        <f t="shared" si="3"/>
         <v>4.3779352153421297E-2</v>
       </c>
       <c r="I8" s="33">
-        <f>J7</f>
+        <f t="shared" si="9"/>
         <v>0.76892333271809798</v>
       </c>
       <c r="J8" s="33">
-        <f>EXP(-A8*H8)</f>
+        <f t="shared" si="4"/>
         <v>0.73605129743954478</v>
       </c>
       <c r="K8" s="43">
-        <f>(I8-J8)/J8</f>
+        <f t="shared" si="5"/>
         <v>4.4659978717384342E-2</v>
       </c>
       <c r="L8" s="40">
-        <f>100*1000000*K8</f>
+        <f t="shared" si="6"/>
         <v>4465997.8717384338</v>
       </c>
       <c r="M8" s="41">
-        <f>L8*J8</f>
+        <f t="shared" si="7"/>
         <v>3287203.5278553199</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:22">
       <c r="A9" s="34">
         <v>8</v>
       </c>
@@ -2485,50 +2500,50 @@
         <v>4.3828314476850198E-2</v>
       </c>
       <c r="C9" s="34">
-        <f>EXP(-B9*A9)</f>
+        <f t="shared" si="0"/>
         <v>0.70424672975993641</v>
       </c>
       <c r="D9" s="39">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E9" s="40">
-        <f>100*1000000*D9</f>
+        <f t="shared" si="1"/>
         <v>4200000</v>
       </c>
       <c r="F9" s="42">
-        <f>C9*E9</f>
+        <f t="shared" si="2"/>
         <v>2957836.2649917328</v>
       </c>
       <c r="G9" s="30">
-        <f>B8</f>
+        <f t="shared" si="8"/>
         <v>4.3779352153421297E-2</v>
       </c>
       <c r="H9" s="30">
-        <f>B9</f>
+        <f t="shared" si="3"/>
         <v>4.3828314476850198E-2</v>
       </c>
       <c r="I9" s="33">
-        <f>J8</f>
+        <f t="shared" si="9"/>
         <v>0.73605129743954478</v>
       </c>
       <c r="J9" s="33">
-        <f>EXP(-A9*H9)</f>
+        <f t="shared" si="4"/>
         <v>0.70424672975993641</v>
       </c>
       <c r="K9" s="43">
-        <f>(I9-J9)/J9</f>
+        <f t="shared" si="5"/>
         <v>4.5161115182529729E-2</v>
       </c>
       <c r="L9" s="40">
-        <f>100*1000000*K9</f>
+        <f t="shared" si="6"/>
         <v>4516111.5182529725</v>
       </c>
       <c r="M9" s="41">
-        <f>L9*J9</f>
+        <f t="shared" si="7"/>
         <v>3180456.7679608371</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:22">
       <c r="A10" s="34">
         <v>9</v>
       </c>
@@ -2536,50 +2551,50 @@
         <v>4.3914561862350203E-2</v>
       </c>
       <c r="C10" s="34">
-        <f>EXP(-B10*A10)</f>
+        <f t="shared" si="0"/>
         <v>0.6735243989025157</v>
       </c>
       <c r="D10" s="39">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E10" s="40">
-        <f>100*1000000*D10</f>
+        <f t="shared" si="1"/>
         <v>4200000</v>
       </c>
       <c r="F10" s="42">
-        <f>C10*E10</f>
+        <f t="shared" si="2"/>
         <v>2828802.475390566</v>
       </c>
       <c r="G10" s="30">
-        <f>B9</f>
+        <f t="shared" si="8"/>
         <v>4.3828314476850198E-2</v>
       </c>
       <c r="H10" s="30">
-        <f>B10</f>
+        <f t="shared" si="3"/>
         <v>4.3914561862350203E-2</v>
       </c>
       <c r="I10" s="33">
-        <f>J9</f>
+        <f t="shared" si="9"/>
         <v>0.70424672975993641</v>
       </c>
       <c r="J10" s="33">
-        <f>EXP(-A10*H10)</f>
+        <f t="shared" si="4"/>
         <v>0.6735243989025157</v>
       </c>
       <c r="K10" s="43">
-        <f>(I10-J10)/J10</f>
+        <f t="shared" si="5"/>
         <v>4.5614280503396262E-2</v>
       </c>
       <c r="L10" s="40">
-        <f>100*1000000*K10</f>
+        <f t="shared" si="6"/>
         <v>4561428.0503396261</v>
       </c>
       <c r="M10" s="41">
-        <f>L10*J10</f>
+        <f t="shared" si="7"/>
         <v>3072233.0857420708</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:22">
       <c r="A11" s="34">
         <v>10</v>
       </c>
@@ -2587,50 +2602,50 @@
         <v>4.4023149444895E-2</v>
       </c>
       <c r="C11" s="34">
-        <f>EXP(-B11*A11)</f>
+        <f t="shared" si="0"/>
         <v>0.64388734748226029</v>
       </c>
       <c r="D11" s="39">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E11" s="40">
-        <f>100*1000000*D11</f>
+        <f t="shared" si="1"/>
         <v>4200000</v>
       </c>
       <c r="F11" s="42">
-        <f>C11*E11</f>
+        <f t="shared" si="2"/>
         <v>2704326.8594254931</v>
       </c>
       <c r="G11" s="30">
-        <f>B10</f>
+        <f t="shared" si="8"/>
         <v>4.3914561862350203E-2</v>
       </c>
       <c r="H11" s="30">
-        <f>B11</f>
+        <f t="shared" si="3"/>
         <v>4.4023149444895E-2</v>
       </c>
       <c r="I11" s="34">
-        <f>J10</f>
+        <f t="shared" si="9"/>
         <v>0.6735243989025157</v>
       </c>
       <c r="J11" s="33">
-        <f>EXP(-A11*H11)</f>
+        <f t="shared" si="4"/>
         <v>0.64388734748226029</v>
       </c>
       <c r="K11" s="43">
-        <f>(I11-J11)/J11</f>
+        <f t="shared" si="5"/>
         <v>4.6028317742447859E-2</v>
       </c>
       <c r="L11" s="40">
-        <f>100*1000000*K11</f>
+        <f t="shared" si="6"/>
         <v>4602831.7742447862</v>
       </c>
       <c r="M11" s="42">
-        <f>L11*J11</f>
+        <f t="shared" si="7"/>
         <v>2963705.1420255415</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:22">
       <c r="E12" s="30" t="s">
         <v>65</v>
       </c>
@@ -2646,7 +2661,7 @@
         <v>35611265.251773968</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:22">
       <c r="L13" s="30" t="s">
         <v>63</v>
       </c>
@@ -2655,7 +2670,7 @@
         <v>2442901.9998463243</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:22">
       <c r="A16" s="36" t="s">
         <v>1</v>
       </c>
@@ -2704,8 +2719,11 @@
       <c r="Q16" s="30" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="S16" s="48"/>
+      <c r="T16" s="48"/>
+      <c r="V16" s="48"/>
+    </row>
+    <row r="17" spans="1:22">
       <c r="A17" s="33">
         <v>1</v>
       </c>
@@ -2720,7 +2738,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E17" s="40">
-        <f>100*1000000*D17</f>
+        <f t="shared" ref="E17:E26" si="10">100*1000000*D17</f>
         <v>4200000</v>
       </c>
       <c r="F17" s="41">
@@ -2731,7 +2749,7 @@
         <v>0.04</v>
       </c>
       <c r="H17" s="45">
-        <f>B17</f>
+        <f t="shared" ref="H17:H26" si="11">B17</f>
         <v>5.2684620000000001E-2</v>
       </c>
       <c r="I17" s="39">
@@ -2739,19 +2757,19 @@
         <v>1</v>
       </c>
       <c r="J17" s="39">
-        <f>EXP(-A17*H17)</f>
+        <f t="shared" ref="J17:J26" si="12">EXP(-A17*H17)</f>
         <v>0.94867915974068651</v>
       </c>
       <c r="K17" s="43">
-        <f>(I17-J17)/J17</f>
+        <f t="shared" ref="K17:K26" si="13">(I17-J17)/J17</f>
         <v>5.4097151531547941E-2</v>
       </c>
       <c r="L17" s="40">
-        <f>100*1000000*K17</f>
+        <f t="shared" ref="L17:L26" si="14">100*1000000*K17</f>
         <v>5409715.1531547941</v>
       </c>
       <c r="M17" s="41">
-        <f>L17*J17</f>
+        <f t="shared" ref="M17:M26" si="15">L17*J17</f>
         <v>5132084.025931349</v>
       </c>
       <c r="O17" s="30">
@@ -2759,15 +2777,17 @@
         <v>4.4001377549850174E-4</v>
       </c>
       <c r="P17" s="30">
-        <f>A2*A2*C2*E2</f>
+        <f>A2*C2*E2</f>
         <v>3986206.0706616333</v>
       </c>
       <c r="Q17" s="30">
         <f>O17*P17</f>
         <v>1753.9855830668726</v>
       </c>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="S17" s="49"/>
+      <c r="T17" s="49"/>
+    </row>
+    <row r="18" spans="1:22">
       <c r="A18" s="33">
         <v>2</v>
       </c>
@@ -2775,62 +2795,64 @@
         <v>4.7382180000000003E-2</v>
       </c>
       <c r="C18" s="33">
-        <f>EXP(-B18*A18)</f>
+        <f t="shared" ref="C18:C26" si="16">EXP(-B18*A18)</f>
         <v>0.90958724435550875</v>
       </c>
       <c r="D18" s="39">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E18" s="40">
-        <f>100*1000000*D18</f>
+        <f t="shared" si="10"/>
         <v>4200000</v>
       </c>
       <c r="F18" s="41">
-        <f>C18*E18</f>
+        <f t="shared" ref="F18:F26" si="17">C18*E18</f>
         <v>3820266.4262931366</v>
       </c>
       <c r="G18" s="45">
-        <f>B17</f>
+        <f t="shared" ref="G18:G26" si="18">B17</f>
         <v>5.2684620000000001E-2</v>
       </c>
       <c r="H18" s="45">
-        <f>B18</f>
+        <f t="shared" si="11"/>
         <v>4.7382180000000003E-2</v>
       </c>
       <c r="I18" s="39">
-        <f>J17</f>
+        <f t="shared" ref="I18:I26" si="19">J17</f>
         <v>0.94867915974068651</v>
       </c>
       <c r="J18" s="39">
-        <f>EXP(-A18*H18)</f>
+        <f t="shared" si="12"/>
         <v>0.90958724435550875</v>
       </c>
       <c r="K18" s="43">
-        <f>(I18-J18)/J18</f>
+        <f t="shared" si="13"/>
         <v>4.2977642472192393E-2</v>
       </c>
       <c r="L18" s="40">
-        <f>100*1000000*K18</f>
+        <f t="shared" si="14"/>
         <v>4297764.2472192394</v>
       </c>
       <c r="M18" s="41">
-        <f>L18*J18</f>
+        <f t="shared" si="15"/>
         <v>3909191.5385177755</v>
       </c>
       <c r="O18" s="30">
-        <f t="shared" ref="O18:O26" si="0">B18-B3</f>
+        <f t="shared" ref="O18:O25" si="20">B18-B3</f>
         <v>-5.220205661317992E-4</v>
       </c>
       <c r="P18" s="30">
-        <f t="shared" ref="P18:P25" si="1">A3*A3*C3*E3</f>
-        <v>15265119.96948193</v>
+        <f t="shared" ref="P18:P25" si="21">A3*C3*E3</f>
+        <v>7632559.9847409651</v>
       </c>
       <c r="Q18" s="30">
-        <f t="shared" ref="Q18:Q26" si="2">O18*P18</f>
-        <v>-7968.7065685387906</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
+        <f t="shared" ref="Q18:Q26" si="22">O18*P18</f>
+        <v>-3984.3532842693953</v>
+      </c>
+      <c r="S18" s="49"/>
+      <c r="T18" s="49"/>
+    </row>
+    <row r="19" spans="1:22">
       <c r="A19" s="33">
         <v>3</v>
       </c>
@@ -2838,62 +2860,64 @@
         <v>4.5085779999999999E-2</v>
       </c>
       <c r="C19" s="33">
-        <f>EXP(-B19*A19)</f>
+        <f t="shared" si="16"/>
         <v>0.87349109856326601</v>
       </c>
       <c r="D19" s="39">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E19" s="40">
-        <f>100*1000000*D19</f>
+        <f t="shared" si="10"/>
         <v>4200000</v>
       </c>
       <c r="F19" s="41">
-        <f>C19*E19</f>
+        <f t="shared" si="17"/>
         <v>3668662.6139657171</v>
       </c>
       <c r="G19" s="45">
-        <f>B18</f>
+        <f t="shared" si="18"/>
         <v>4.7382180000000003E-2</v>
       </c>
       <c r="H19" s="45">
-        <f>B19</f>
+        <f t="shared" si="11"/>
         <v>4.5085779999999999E-2</v>
       </c>
       <c r="I19" s="39">
-        <f>J18</f>
+        <f t="shared" si="19"/>
         <v>0.90958724435550875</v>
       </c>
       <c r="J19" s="39">
-        <f>EXP(-A19*H19)</f>
+        <f t="shared" si="12"/>
         <v>0.87349109856326601</v>
       </c>
       <c r="K19" s="43">
-        <f>(I19-J19)/J19</f>
+        <f t="shared" si="13"/>
         <v>4.1323999582381934E-2</v>
       </c>
       <c r="L19" s="40">
-        <f>100*1000000*K19</f>
+        <f t="shared" si="14"/>
         <v>4132399.9582381933</v>
       </c>
       <c r="M19" s="41">
-        <f>L19*J19</f>
+        <f t="shared" si="15"/>
         <v>3609614.579224274</v>
       </c>
       <c r="O19" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="20"/>
         <v>-3.4355760259130452E-4</v>
       </c>
       <c r="P19" s="30">
-        <f t="shared" si="1"/>
-        <v>32983950.339761354</v>
+        <f t="shared" si="21"/>
+        <v>10994650.113253785</v>
       </c>
       <c r="Q19" s="30">
-        <f t="shared" si="2"/>
-        <v>-11331.886902719056</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17">
+        <f t="shared" si="22"/>
+        <v>-3777.2956342396851</v>
+      </c>
+      <c r="S19" s="49"/>
+      <c r="T19" s="49"/>
+    </row>
+    <row r="20" spans="1:22">
       <c r="A20" s="33">
         <v>4</v>
       </c>
@@ -2901,62 +2925,64 @@
         <v>4.420698E-2</v>
       </c>
       <c r="C20" s="33">
-        <f>EXP(-B20*A20)</f>
+        <f t="shared" si="16"/>
         <v>0.83792396207299524</v>
       </c>
       <c r="D20" s="39">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E20" s="40">
-        <f>100*1000000*D20</f>
+        <f t="shared" si="10"/>
         <v>4200000</v>
       </c>
       <c r="F20" s="41">
-        <f>C20*E20</f>
+        <f t="shared" si="17"/>
         <v>3519280.6407065801</v>
       </c>
       <c r="G20" s="45">
-        <f>B19</f>
+        <f t="shared" si="18"/>
         <v>4.5085779999999999E-2</v>
       </c>
       <c r="H20" s="45">
-        <f>B20</f>
+        <f t="shared" si="11"/>
         <v>4.420698E-2</v>
       </c>
       <c r="I20" s="39">
-        <f>J19</f>
+        <f t="shared" si="19"/>
         <v>0.87349109856326601</v>
       </c>
       <c r="J20" s="39">
-        <f>EXP(-A20*H20)</f>
+        <f t="shared" si="12"/>
         <v>0.83792396207299524</v>
       </c>
       <c r="K20" s="43">
-        <f>(I20-J20)/J20</f>
+        <f t="shared" si="13"/>
         <v>4.2446735145607831E-2</v>
       </c>
       <c r="L20" s="40">
-        <f>100*1000000*K20</f>
+        <f t="shared" si="14"/>
         <v>4244673.5145607833</v>
       </c>
       <c r="M20" s="41">
-        <f>L20*J20</f>
+        <f t="shared" si="15"/>
         <v>3556713.649027077</v>
       </c>
       <c r="O20" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="20"/>
         <v>-1.3777025634260226E-4</v>
       </c>
       <c r="P20" s="30">
-        <f t="shared" si="1"/>
-        <v>56277468.259361185</v>
+        <f t="shared" si="21"/>
+        <v>14069367.064840296</v>
       </c>
       <c r="Q20" s="30">
-        <f t="shared" si="2"/>
-        <v>-7753.3612284048522</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17">
+        <f t="shared" si="22"/>
+        <v>-1938.3403071012131</v>
+      </c>
+      <c r="S20" s="49"/>
+      <c r="T20" s="49"/>
+    </row>
+    <row r="21" spans="1:22">
       <c r="A21" s="34">
         <v>5</v>
       </c>
@@ -2964,62 +2990,64 @@
         <v>4.3660200000000003E-2</v>
       </c>
       <c r="C21" s="34">
-        <f>EXP(-B21*A21)</f>
+        <f t="shared" si="16"/>
         <v>0.80388343633224801</v>
       </c>
       <c r="D21" s="39">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E21" s="40">
-        <f>100*1000000*D21</f>
+        <f t="shared" si="10"/>
         <v>4200000</v>
       </c>
       <c r="F21" s="42">
-        <f>C21*E21</f>
+        <f t="shared" si="17"/>
         <v>3376310.4325954416</v>
       </c>
       <c r="G21" s="45">
-        <f>B20</f>
+        <f t="shared" si="18"/>
         <v>4.420698E-2</v>
       </c>
       <c r="H21" s="45">
-        <f>B21</f>
+        <f t="shared" si="11"/>
         <v>4.3660200000000003E-2</v>
       </c>
       <c r="I21" s="39">
-        <f>J20</f>
+        <f t="shared" si="19"/>
         <v>0.83792396207299524</v>
       </c>
       <c r="J21" s="39">
-        <f>EXP(-A21*H21)</f>
+        <f t="shared" si="12"/>
         <v>0.80388343633224801</v>
       </c>
       <c r="K21" s="43">
-        <f>(I21-J21)/J21</f>
+        <f t="shared" si="13"/>
         <v>4.2345101543649857E-2</v>
       </c>
       <c r="L21" s="40">
-        <f>100*1000000*K21</f>
+        <f t="shared" si="14"/>
         <v>4234510.1543649854</v>
       </c>
       <c r="M21" s="41">
-        <f>L21*J21</f>
+        <f t="shared" si="15"/>
         <v>3404052.5740747224</v>
       </c>
       <c r="O21" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="20"/>
         <v>-2.6777468253010028E-4</v>
       </c>
       <c r="P21" s="30">
-        <f t="shared" si="1"/>
-        <v>84294825.128274232</v>
+        <f t="shared" si="21"/>
+        <v>16858965.025654845</v>
       </c>
       <c r="Q21" s="30">
-        <f t="shared" si="2"/>
-        <v>-22572.020037653954</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17">
+        <f t="shared" si="22"/>
+        <v>-4514.4040075307903</v>
+      </c>
+      <c r="S21" s="49"/>
+      <c r="T21" s="49"/>
+    </row>
+    <row r="22" spans="1:22">
       <c r="A22" s="34">
         <v>6</v>
       </c>
@@ -3027,62 +3055,64 @@
         <v>4.3534870000000003E-2</v>
       </c>
       <c r="C22" s="34">
-        <f>EXP(-B22*A22)</f>
+        <f t="shared" si="16"/>
         <v>0.77011977829865819</v>
       </c>
       <c r="D22" s="39">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E22" s="40">
-        <f>100*1000000*D22</f>
+        <f t="shared" si="10"/>
         <v>4200000</v>
       </c>
       <c r="F22" s="42">
-        <f>C22*E22</f>
+        <f t="shared" si="17"/>
         <v>3234503.0688543646</v>
       </c>
       <c r="G22" s="45">
-        <f>B21</f>
+        <f t="shared" si="18"/>
         <v>4.3660200000000003E-2</v>
       </c>
       <c r="H22" s="45">
-        <f>B22</f>
+        <f t="shared" si="11"/>
         <v>4.3534870000000003E-2</v>
       </c>
       <c r="I22" s="39">
-        <f>J21</f>
+        <f t="shared" si="19"/>
         <v>0.80388343633224801</v>
       </c>
       <c r="J22" s="39">
-        <f>EXP(-A22*H22)</f>
+        <f t="shared" si="12"/>
         <v>0.77011977829865819</v>
       </c>
       <c r="K22" s="43">
-        <f>(I22-J22)/J22</f>
+        <f t="shared" si="13"/>
         <v>4.3842086627329843E-2</v>
       </c>
       <c r="L22" s="40">
-        <f>100*1000000*K22</f>
+        <f t="shared" si="14"/>
         <v>4384208.6627329839</v>
       </c>
       <c r="M22" s="41">
-        <f>L22*J22</f>
+        <f t="shared" si="15"/>
         <v>3376365.8033589823</v>
       </c>
       <c r="O22" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="20"/>
         <v>-2.591319703819997E-4</v>
       </c>
       <c r="P22" s="30">
-        <f t="shared" si="1"/>
-        <v>116261207.9069764</v>
+        <f t="shared" si="21"/>
+        <v>19376867.984496068</v>
       </c>
       <c r="Q22" s="30">
-        <f t="shared" si="2"/>
-        <v>-30126.99588392612</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17">
+        <f t="shared" si="22"/>
+        <v>-5021.165980654353</v>
+      </c>
+      <c r="S22" s="49"/>
+      <c r="T22" s="49"/>
+    </row>
+    <row r="23" spans="1:22">
       <c r="A23" s="34">
         <v>7</v>
       </c>
@@ -3090,62 +3120,64 @@
         <v>4.3780769999999997E-2</v>
       </c>
       <c r="C23" s="34">
-        <f>EXP(-B23*A23)</f>
+        <f t="shared" si="16"/>
         <v>0.73604399222109995</v>
       </c>
       <c r="D23" s="39">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E23" s="40">
-        <f>100*1000000*D23</f>
+        <f t="shared" si="10"/>
         <v>4200000</v>
       </c>
       <c r="F23" s="42">
-        <f>C23*E23</f>
+        <f t="shared" si="17"/>
         <v>3091384.76732862</v>
       </c>
       <c r="G23" s="45">
-        <f>B22</f>
+        <f t="shared" si="18"/>
         <v>4.3534870000000003E-2</v>
       </c>
       <c r="H23" s="45">
-        <f>B23</f>
+        <f t="shared" si="11"/>
         <v>4.3780769999999997E-2</v>
       </c>
       <c r="I23" s="39">
-        <f>J22</f>
+        <f t="shared" si="19"/>
         <v>0.77011977829865819</v>
       </c>
       <c r="J23" s="39">
-        <f>EXP(-A23*H23)</f>
+        <f t="shared" si="12"/>
         <v>0.73604399222109995</v>
       </c>
       <c r="K23" s="43">
-        <f>(I23-J23)/J23</f>
+        <f t="shared" si="13"/>
         <v>4.6295855190299849E-2</v>
       </c>
       <c r="L23" s="40">
-        <f>100*1000000*K23</f>
+        <f t="shared" si="14"/>
         <v>4629585.5190299852</v>
       </c>
       <c r="M23" s="41">
-        <f>L23*J23</f>
+        <f t="shared" si="15"/>
         <v>3407578.6077558235</v>
       </c>
       <c r="O23" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="20"/>
         <v>1.4178465786995886E-6</v>
       </c>
       <c r="P23" s="30">
-        <f t="shared" si="1"/>
-        <v>151479357.0130583</v>
+        <f t="shared" si="21"/>
+        <v>21639908.144722618</v>
       </c>
       <c r="Q23" s="30">
-        <f t="shared" si="2"/>
-        <v>214.77448808457825</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17">
+        <f t="shared" si="22"/>
+        <v>30.682069726368326</v>
+      </c>
+      <c r="S23" s="49"/>
+      <c r="T23" s="49"/>
+    </row>
+    <row r="24" spans="1:22">
       <c r="A24" s="34">
         <v>8</v>
       </c>
@@ -3153,62 +3185,64 @@
         <v>4.406587E-2</v>
       </c>
       <c r="C24" s="34">
-        <f>EXP(-B24*A24)</f>
+        <f t="shared" si="16"/>
         <v>0.70290961911193262</v>
       </c>
       <c r="D24" s="39">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E24" s="40">
-        <f>100*1000000*D24</f>
+        <f t="shared" si="10"/>
         <v>4200000</v>
       </c>
       <c r="F24" s="42">
-        <f>C24*E24</f>
+        <f t="shared" si="17"/>
         <v>2952220.400270117</v>
       </c>
       <c r="G24" s="45">
-        <f>B23</f>
+        <f t="shared" si="18"/>
         <v>4.3780769999999997E-2</v>
       </c>
       <c r="H24" s="45">
-        <f>B24</f>
+        <f t="shared" si="11"/>
         <v>4.406587E-2</v>
       </c>
       <c r="I24" s="39">
-        <f>J23</f>
+        <f t="shared" si="19"/>
         <v>0.73604399222109995</v>
       </c>
       <c r="J24" s="39">
-        <f>EXP(-A24*H24)</f>
+        <f t="shared" si="12"/>
         <v>0.70290961911193262</v>
       </c>
       <c r="K24" s="43">
-        <f>(I24-J24)/J24</f>
+        <f t="shared" si="13"/>
         <v>4.7138881313119371E-2</v>
       </c>
       <c r="L24" s="40">
-        <f>100*1000000*K24</f>
+        <f t="shared" si="14"/>
         <v>4713888.1313119372</v>
       </c>
       <c r="M24" s="41">
-        <f>L24*J24</f>
+        <f t="shared" si="15"/>
         <v>3313437.3109167335</v>
       </c>
       <c r="O24" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="20"/>
         <v>2.3755552314980166E-4</v>
       </c>
       <c r="P24" s="30">
-        <f t="shared" si="1"/>
-        <v>189301520.9594709</v>
+        <f t="shared" si="21"/>
+        <v>23662690.119933862</v>
       </c>
       <c r="Q24" s="30">
-        <f t="shared" si="2"/>
-        <v>44969.621844580251</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17">
+        <f t="shared" si="22"/>
+        <v>5621.2027305725314</v>
+      </c>
+      <c r="S24" s="49"/>
+      <c r="T24" s="49"/>
+    </row>
+    <row r="25" spans="1:22">
       <c r="A25" s="34">
         <v>9</v>
       </c>
@@ -3216,62 +3250,64 @@
         <v>4.4304950000000003E-2</v>
       </c>
       <c r="C25" s="34">
-        <f>EXP(-B25*A25)</f>
+        <f t="shared" si="16"/>
         <v>0.67116212782262019</v>
       </c>
       <c r="D25" s="39">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E25" s="40">
-        <f>100*1000000*D25</f>
+        <f t="shared" si="10"/>
         <v>4200000</v>
       </c>
       <c r="F25" s="42">
-        <f>C25*E25</f>
+        <f t="shared" si="17"/>
         <v>2818880.9368550046</v>
       </c>
       <c r="G25" s="45">
-        <f>B24</f>
+        <f t="shared" si="18"/>
         <v>4.406587E-2</v>
       </c>
       <c r="H25" s="45">
-        <f>B25</f>
+        <f t="shared" si="11"/>
         <v>4.4304950000000003E-2</v>
       </c>
       <c r="I25" s="39">
-        <f>J24</f>
+        <f t="shared" si="19"/>
         <v>0.70290961911193262</v>
       </c>
       <c r="J25" s="39">
-        <f>EXP(-A25*H25)</f>
+        <f t="shared" si="12"/>
         <v>0.67116212782262019</v>
       </c>
       <c r="K25" s="43">
-        <f>(I25-J25)/J25</f>
+        <f t="shared" si="13"/>
         <v>4.7302268666897858E-2</v>
       </c>
       <c r="L25" s="40">
-        <f>100*1000000*K25</f>
+        <f t="shared" si="14"/>
         <v>4730226.8666897854</v>
       </c>
       <c r="M25" s="41">
-        <f>L25*J25</f>
+        <f t="shared" si="15"/>
         <v>3174749.128931242</v>
       </c>
       <c r="O25" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="20"/>
         <v>3.9038813764979974E-4</v>
       </c>
       <c r="P25" s="30">
-        <f t="shared" si="1"/>
-        <v>229133000.50663584</v>
+        <f t="shared" si="21"/>
+        <v>25459222.278515093</v>
       </c>
       <c r="Q25" s="30">
-        <f t="shared" si="2"/>
-        <v>89450.805341896194</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17">
+        <f t="shared" si="22"/>
+        <v>9938.9783713217985</v>
+      </c>
+      <c r="S25" s="49"/>
+      <c r="T25" s="49"/>
+    </row>
+    <row r="26" spans="1:22">
       <c r="A26" s="34">
         <v>10</v>
       </c>
@@ -3279,46 +3315,46 @@
         <v>4.4471370000000003E-2</v>
       </c>
       <c r="C26" s="34">
-        <f>EXP(-B26*A26)</f>
+        <f t="shared" si="16"/>
         <v>0.6410077702884962</v>
       </c>
       <c r="D26" s="39">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E26" s="40">
-        <f>100*1000000*D26</f>
+        <f t="shared" si="10"/>
         <v>4200000</v>
       </c>
       <c r="F26" s="42">
-        <f>C26*E26</f>
+        <f t="shared" si="17"/>
         <v>2692232.6352116843</v>
       </c>
       <c r="G26" s="45">
-        <f>B25</f>
+        <f t="shared" si="18"/>
         <v>4.4304950000000003E-2</v>
       </c>
       <c r="H26" s="45">
-        <f>B26</f>
+        <f t="shared" si="11"/>
         <v>4.4471370000000003E-2</v>
       </c>
       <c r="I26" s="46">
-        <f>J25</f>
+        <f t="shared" si="19"/>
         <v>0.67116212782262019</v>
       </c>
       <c r="J26" s="39">
-        <f>EXP(-A26*H26)</f>
+        <f t="shared" si="12"/>
         <v>0.6410077702884962</v>
       </c>
       <c r="K26" s="43">
-        <f>(I26-J26)/J26</f>
+        <f t="shared" si="13"/>
         <v>4.7042109209616163E-2</v>
       </c>
       <c r="L26" s="40">
-        <f>100*1000000*K26</f>
+        <f t="shared" si="14"/>
         <v>4704210.9209616166</v>
       </c>
       <c r="M26" s="42">
-        <f>L26*J26</f>
+        <f t="shared" si="15"/>
         <v>3015435.753412399</v>
       </c>
       <c r="O26" s="30">
@@ -3326,15 +3362,16 @@
         <v>4.482205551050028E-4</v>
       </c>
       <c r="P26" s="30">
-        <f>A11*A11*C11*E11+100000000</f>
-        <v>370432685.94254935</v>
+        <f>A11*C11*(E11+100*1000000)</f>
+        <v>670930616.0765152</v>
       </c>
       <c r="Q26" s="30">
-        <f t="shared" si="2"/>
-        <v>166035.54412220663</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17">
+        <f>O26*P26</f>
+        <v>300724.89317475713</v>
+      </c>
+      <c r="T26" s="49"/>
+    </row>
+    <row r="27" spans="1:22">
       <c r="E27" s="30" t="s">
         <v>65</v>
       </c>
@@ -3349,8 +3386,9 @@
         <f>SUM(M17:M26)</f>
         <v>35899222.971150376</v>
       </c>
-    </row>
-    <row r="28" spans="1:17">
+      <c r="T27" s="48"/>
+    </row>
+    <row r="28" spans="1:22">
       <c r="L28" s="30" t="s">
         <v>63</v>
       </c>
@@ -3359,7 +3397,7 @@
         <v>2741028.5781588294</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:22">
       <c r="L29" s="30" t="s">
         <v>71</v>
       </c>
@@ -3372,8 +3410,9 @@
       </c>
       <c r="Q29" s="47">
         <f>SUM(Q17:Q26)</f>
-        <v>222671.76075859176</v>
-      </c>
+        <v>298834.18271564925</v>
+      </c>
+      <c r="V29" s="50"/>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="30" t="s">

</xml_diff>